<commit_message>
List of AI bills from 116-119 Congress
</commit_message>
<xml_diff>
--- a/ai_bills.xlsx
+++ b/ai_bills.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7410,6 +7410,3066 @@
         </is>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>HB5685</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Securing American Leadership in Science and Technology Act of 2020</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Extends through FY2029 the Office of Science and Technology Policy (OSTP), the Office of Science of the Department of Energy, the Advanced Research Projects Agency-Energy, the National Institute of Standards and Technology (NIST), the National Oceanic and Atmospheric Administration, and the National Science Foundation (NSF). The bill sets forth programs, projects, and activities, including those regarding federal research security, the science and technical workforce, basic energy sciences research and upgrades to certain facilities, computational materials and chemistry science, advanced scientific computing, high energy physics, biological systems science and environmental science, fusion energy sciences research, nuclear physics, carbon utilization research infrastructure, enhanced geothermal energy, quantum information science and technology research, cybersecurity research, artificial intelligence and data science, engineering biology research, next generation digital radar, Antarctic nongovernmental activities and environmental liability requirements, and federal government inventions. The OSTP shall submit a comprehensive national science and technology strategy, and complete a review of U.S. science and technology enterprise. The Office of Science shall continue to leverage U.S. participation in the Large Hadron Collider, prioritize international partnerships and investments in the Long-Baseline Neutrino Facility/Deep Underground Neutrino Experiment, and prioritize international collaboration that would provide U.S. researchers access to the most advanced accelerator facilities in the world. The Government Accountability Office shall evaluate NIST's Center for Neutron Research. The NSF shall contract the National Academy of Public Administration to study the organizational and management structure of the NSF.</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>1</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2020-01-28</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB5685/2019</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/5685/all-info</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Frank Lucas</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>HR153</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Supporting the development of guidelines for ethical development of artificial intelligence.</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>This resolution supports the development of guidelines for the ethical development of artificial intelligence, with aims including engagement among industry, government, academia, and civil society.</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>2019-02-27</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HR153/2019</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-resolution/153/all-info</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Brenda Lawrence</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>SB2637</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Mind Your Own Business Act of 2019</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Requires assessments, periodic reporting, and the development of an opt-out process for specified commercial entities that operate high-risk information systems or automated-decision systems, such as those that use artificial intelligence or machine learning. An automated-decision system or information system is considered high risk if it (1) raises security or privacy concerns; (2) involves the personal information of a significant number of people; or (3) systematically monitors a large, publicly-accessible physical location. An automated-decision system is also considered high risk if it (1) may contribute to inaccuracy, bias, or discrimination or (2) facilitates decision-making about sensitive aspects of consumers' lives by evaluating their behavior.Covered commercial entities must assess such high-risk systems and evaluate the extent to which they protect against the risk of exposing personal information. The bill further requires certain larger commercial entities to submit an annual report for which corporate officers must certify that the entity is in compliance with the Federal Trade Commission's (FTC) implementing regulations. A failure to comply with the reporting requirements is subject to criminal penalties and excise tax.Among other provisions, the bill requires the FTC to create a web portal for consumers to opt out of data sharing and view their opt-out status. Opting out prevents covered commercial entities from sharing personal information with third parties.The bill increases the civil penalties for unfair trade practices, which the bill modifies to include practices that involve noneconomic impacts or create a significant risk of exposing personal information.</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2019-10-17</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2637/2019</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/2637/all-info</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Ron Wyden</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>HB7339</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>AI Careers Act of 2020</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>To direct the Director of the National Institute of Technologies to undertake certain activities with respect to the artificial intelligence workforce, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>2020-06-25</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7339/2019</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/7339/all-info</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Steve Cohen</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>SB4700</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>A bill to establish a Center for Artificial Intelligence of the National Oceanic and Atmospheric Administration, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Directs the National Oceanic Atmospheric Administration (NOAA) to establish a Center for Artificial Intelligence. The goals of the center must be to (1) coordinate and facilitate scientific and technological efforts relating to artificial intelligence across NOAA, and (2) expand external partnerships and build workforce proficiency to effectively transition artificial intelligence research and applications to operations. Through the center, NOAA must implement a comprehensive program to improve the use of artificial intelligence systems in support of its mission.</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>2020-09-24</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB4700/2019</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/4700/all-info</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Cory Gardner</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>SB5043</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>American COMPETE Act of 2020 American Competitiveness Of a More Productive Emerging Tech Economy Act of 2020</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Requires the Department of Commerce and the Federal Trade Commission to study and submit reports on the state of specified technology industries (e.g., artificial intelligence, quantum computing, blockchain technology, and unmanned delivery services) and the impact of these industries on the U.S. economy.</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>1</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2020-12-17</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB5043/2019</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/5043/all-info</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Deb Fischer</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>SB3965</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence for the Armed Forces Act of 2020</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>A bill to accelerate the application of artificial intelligence in the Department of Defense and to strengthen the workforce that pertains to artificial intelligence, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>2020-06-16</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3965/2019</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3965/all-info</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Martin Heinrich</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>HB7007</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Compensation for Americans Act of 2020</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Requires the Department of State to negotiate with China to secure compensation for China's distortion of information related to the spread of COVID-19 (i.e., coronavirus disease 2019). The bill also contains other China-related provisions, such as those imposing sanctions on certain Chinese individuals and entities. As part of such negotiations, the President shall (1) freeze Chinese assets subject to U.S. jurisdiction; (2) suspend the required review of any proposed acquisition of a U.S. entity by a Chinese entity; (3) impose sanctions on Chinese entities in certain industries, such as artificial intelligence and pharmaceuticals; (4) impose sanctions on various individuals, including Chinese government officials and Chinese citizens responsible for stealing intellectual property from U.S. entities; and (5) prohibit using federal funds to procure goods manufactured or sourced from a Chinese company, if such goods pose a supply chain risk to U.S. national security. The President s may terminate such prohibitions and sanctions if China and the United States come to an agreement regarding compensation related to COVID-19. The Department of the Treasury shall establish a public repository with information about entities that are owned, financed, or controlled by the Chinese government. Other provisions in this bill include (1) imposing export controls on telecommunications equipment that would help China carry out censorship or surveillance, (2) banning researchers affiliated with China's military from obtaining visas, and (3) requiring U.S. World Bank representatives to end China's eligibility for World Bank assistance.</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>2020-05-22</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7007/2019</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/7007/all-info</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Ann Wagner</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>SB1108</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Algorithmic Accountability Act of 2019</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Requires specified commercial entities to conduct assessments of high-risk systems that involve personal information or make automated decisions, such as systems that use artificial intelligence or machine learning.Specifically, high-risk automated decision systems include those that (1) may contribute to inaccuracy, bias, or discrimination; or (2) facilitate decision-making about sensitive aspects of consumers' lives by evaluating consumers' behavior. Further, an automated-decision system, or information system involving personal data, is considered high-risk if it (1) raises security or privacy concerns, (2) involves the personal information of a significant number of people, or (3) systematically monitors a large, publicly accessible physical location.Assessments of high-risk automated-decision systems must (1) describe the system in detail, (2) assess the relative costs and benefits of the system, (3) determine the risks to the privacy and security of personal information, and (4) explain the steps taken to minimize those risks, if discovered. Assessments of high-risk information systems involving personal information must evaluate the extent to which the system protects the privacy and security of such information.</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>2019-04-10</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1108/2019</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/1108/all-info</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Ron Wyden</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>SB1558</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>AI–IA Artificial Intelligence Initiative Act</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Requires certain federal activities related to artificial intelligence, including implementation by the President of a National Artificial Intelligence Research and Development Initiative. The initiative must invest in artificial intelligence research and development and support the development of an artificial intelligence science and technology workforce pipeline, among other activities. The Office of Science and Technology Policy (OSTP) shall establish or designate a National Artificial Intelligence Advisory Committee to advise the OSTP on matters related to the initiative; a National Artificial Intelligence Coordination Office to provide technical and administrative support to the advisory committee and serve as the point of contact on federal artificial intelligence activities; and an Interagency Committee on Artificial Intelligence to coordinate the artificial intelligence and technology research and education activities and programs of the federal agencies, among other activities. The National Institute of Standards and Technology shall, among other things carry out initiative activities, including by awarding contracts as necessary; support the development of measurements and standards necessary to advance commercial development of artificial intelligence applications; and establish collaborative ventures or consortia. The National Science Foundation shall implement a research and education program on artificial intelligence and engineering, and award grants to establish up to five Multidisciplinary Centers for Artificial Intelligence Research and Education to conduct activities in support of the initiative. The Department of Energy shall carry out an artificial intelligence research and development program.</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>2019-05-21</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1558/2019</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/1558/all-info</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Martin Heinrich</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>HB1025</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>UIGHUR Act of 2019 Uighur Intervention and Global Humanitarian Unified Response Act of 2019</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Imposes sourcing restrictions and export controls related to China's mass detention of the Uyghurs, a predominantly Muslim Turkic ethnic group in Xinjiang province. Executive agencies shall not procure goods or services from foreign persons who in the last three years substantially facilitated or knowingly assisted such mass detention. When procuring goods or services from U.S. persons, executive agencies shall provide adverse consideration to awarding contracts to those involved with such mass detention, and assess the availability of other sources. The President may waive these restrictions for national security or national interest purposes. The Department of Commerce shall deny applications to export to China various technologies, including those related to artificial intelligence or biometrics, unless the applicant certifies that the technology will not be knowingly used to facilitate the mass detention of Turkic Muslims. The Department of State shall ensure that certain U.S. diplomatic facilities in China can provide services in the Uyghur language. The State Department shall establish a website for reporting harassment or surveillance of persons in the United States by Chinese representatives or agents, and procedures for sharing such reports with law enforcement agencies. directs various agencies to report on specified topics, including China's development of technologies related to mass detection and surveillance.</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>2019-02-06</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB1025/2019</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/1025/all-info</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Brad Sherman</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>SB143</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Department of Energy Veterans’ Health Initiative Act</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Directs the Department of Energy (DOE) to establish a research program in artificial intelligence and high-performance computing that is focused on the development of tools to (1) solve big data challenges associated with veterans' health care, and (2) support the Department of Veterans Affairs in identifying potential health risks and challenges. DOE shall carry out a pilot program to develop tools for big data analytics in order to advance artificial intelligence technologies to solve complex big data challenges.</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>2019-01-16</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB143/2019</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/143/all-info</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Joni Ernst</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>HB2432</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Future DATA Act Future Defense Artificial Intelligence Technology Assessment Act</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Directs the Department of Defense (DOD) to report on its artificial intelligence (AI) strategy. The report shall include an analysis of the increasing use of AI by DOD, identification of any data gaps, identification of applicable ethical guidelines, plans to protect systems from bad actors, expected benefits of AI for Armed Forces operations, and plans for collaboration.</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>1</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>2019-05-01</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2432/2019</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/2432/all-info</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Neal Dunn</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>SB4049</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>National Defense Authorization Act for Fiscal Year 2021</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Authorizes FY2021 appropriations and sets forth policies for Department of Defense (DOD) programs and activities, including military personnel strengths. It does not provide budget authority, which is provided in subsequent appropriations legislation. The bill authorizes appropriations to DOD for Procurement, including aircraft, weapons and tracked combat vehicles, shipbuilding and conversion, and missiles; Research, Development, Test, and Evaluation; Operation and Maintenance; Working Capital Funds; Chemical Agents and Munitions Destruction; Drug Interdiction and Counter-Drug Activities; the Defense Inspector General; the Defense Health Program; the Armed Forces Retirement Home; Overseas Contingency Operations; and Military Construction. The bill authorizes the FY2021 personnel strengths for active duty and reserve forces and sets forth policies, including those regarding military personnel; acquisition policy and management; transfer of property for law enforcement activities; financial oversight; Space Force matters; artificial intelligence; advanced microelectronics; international programs; nuclear security and energy; National Guard and Reserve Forces facilities; compensation and other personnel benefits; health care; DOD organization and management; civilian personnel matters; diversity and inclusion; matters relating to foreign nations; hostage recovery; emergency alert systems; the autonomy of Hong Kong; and strategic programs, cyber, and intelligence matters. The bill authorizes appropriations for base realignment and closure activities, and maritime matters. The bill authorizes various intelligence-related activities and programs for FY2021. The bill also authorizes appropriations and sets forth policies for Department of Energy national security programs, including the National Nuclear Security Administration and the Defense Nuclear Facilities Safety Board.</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>2</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>2020-08-07</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB4049/2019</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/4049/all-info</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>James Inhofe</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>HR1250</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Expressing the sense of the House of Representatives with respect to the principles that should guide the national artificial intelligence strategy of the United States.</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Expressing the sense of the House of Representatives with respect to the principles that should guide the national artificial intelligence strategy of the United States.</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>2020-12-04</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HR1250/2019</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-resolution/1250/all-info</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>Will Hurd</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>SB3722</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>EMPIL-DOC Act Expanding Medical Partnerships with Israel to Lessen Dependence On China Act</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Authorizes a bilateral grant program with Israel to develop health technologies, with an emphasis on the use of technology, personalized medicine, and data in relation to COVID-19 (i.e., coronavirus disease 2019). Technologies to be developed through this program include, among others, artificial intelligence, respiratory assist devices, and diagnostic tests. In addition, the program conditions funding on a matching contribution from the government of Israel.</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>2020-05-13</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3722/2019</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3722/all-info</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Ted Cruz</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>SB1363</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>AI in Government Act of 2019</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Establishes the AI Center of Excellence within the General Services Administration to advise and promote the efforts of the federal government in developing innovative uses of artificial intelligence (AI) to benefit the public, and improve cohesion and competency in the use of AI. The Office of Management and Budget must issue a memorandum to federal agencies regarding AI governance approaches, to be followed by preparation and submission of governance plans by the agencies. In addition, the Office of Personnel Management must identify key skills and competencies needed for positions related to AI; and establish an occupational series, or revise an existing job series, to include positions the primary duties of which relate to AI.</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>2019-05-08</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1363/2019</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/1363/all-info</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Brian Schatz</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>HB6216</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>National Artificial Intelligence Initiative Act of 2020</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>To establish the National Artificial Intelligence Initiative, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>1</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>2020-03-12</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6216/2019</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6216/all-info</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Eddie Johnson</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>HB2202</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>GrAITR Act Growing Artificial Intelligence Through Research Act</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Requires certain federal activities related to artificial intelligence, including implementation by the President of a National Artificial Intelligence Initiative. The initiative must invest in artificial intelligence research and support the development of an artificial intelligence science and technology workforce pipeline, among other activities. The Office of Science and Technology Policy (OSTP) shall establish or designate a National Artificial Intelligence Advisory Committee to advise the OSTP on matters related to the initiative; a National Artificial Intelligence Coordination Office to provide technical and administrative support to the advisory committee and serve as the point of contact on federal artificial intelligence activities; and an Interagency Committee on Artificial Intelligence to coordinate the artificial intelligence and technology research and education activities and programs of the federal agencies, among other activities. The National Institute of Standards and Technology shall, among other things carry out initiative activities, including by awarding contracts as necessary; support the development of measurements and standards necessary to advance commercial development of artificial intelligence applications; and establish collaborative ventures or consortia. The National Science Foundation shall implement a research and education program on artificial intelligence and engineering, and award grants to establish up to five Multidisciplinary Centers for Artificial Intelligence Research and Education to conduct activities in support of the initiative. The Department of Energy shall carry out an artificial intelligence research program.</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>1</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>2019-04-10</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2202/2019</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/2202/all-info</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Daniel Lipinski</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>HB2613</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Advancing Innovation to Assist Law Enforcement Act</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Requires the Financial Crimes Enforcement Network to report on emerging financial technologies—including artificial intelligence, digital identity, and blockchain technologies—and their use in law enforcement.</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>2</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>2019-09-23</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2613/2019</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/2613/all-info</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Anthony Gonzalez</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>SB2763</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Filter Bubble Transparency Act</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Establishes requirements for large online platforms that use algorithms applying artificial intelligence or machine learning to user-specific data to determine the manner in which content is displayed to users. Specifically, if an online platform applies such techniques to user-specific data that is not expressly provided by the user, the platform must (1) notify users that the platform uses such data, and (2) make a version of the platform available that uses only user-specific data that has been expressly provided by the user and which enables users to switch between the two platforms. These requirements do not apply to search engines operated by downstream providers with fewer than 1,000 employees and that have an agreement to access an index of web pages from an upstream provider. However, the bill requires such upstream providers to make their algorithm available to downstream providers as part of such an agreement.</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>2019-10-31</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2763/2019</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/2763/all-info</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>John Thune</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>HB6978</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Endless Frontier Act</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Redesignates the National Science Foundation as the National Science and Technology Foundation and establishes a Directorate for Technology within the foundation. The goals of the directorate shall be to (1) strengthen U.S. leadership in critical technologies through fundamental research in key technology focus areas, such as artificial intelligence, high-performance computing, and advanced manufacturing; (2) enhance U.S. competitiveness in the focus areas by improving education in such areas and attracting more students to such areas; and (3) foster the impact of federally funded research and development through accelerated translation of advances in the focus areas into processes and products that help achieve national goals. The Department of Commerce shall carry out a program to designate and support eligible consortia as regional technology hubs that facilitate activities that (1) enable U.S. leadership in a key technology focus area, and (2) support regional economic development that diffuses innovation capacity around the United States. The Office of Science and Technology Policy, Commerce, the National Security Council, and other relevant federal agencies shall (1) review the national security strategy and programs and resources pertaining to U.S. national competitiveness in science, research, and innovation to support such strategy; and (2) develop a strategy for the federal government to improve such competitiveness to support the national security strategy.</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>2020-05-22</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6978/2019</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6978/all-info</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>Ro Khanna</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>HB7559</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>FUTURE of Artificial Intelligence Act of 2020 Fundamentally Understanding The Usability and Realistic Evolution of Artificial Intelligence Act of 2020</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>To require the Director of the National Science Foundation, in consultation with the Director of the Office of Science and Technology Policy, to establish an advisory committee to advise the President on matters relating to the development of artificial intelligence, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>2020-07-09</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7559/2019</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/7559/all-info</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>Pete Olson</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>SB3891</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Advancing Artificial Intelligence Research Act of 2020</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>A bill to require the Director of the National Institute of Standards and Technology to advance the development of technical standards for artificial intelligence, to establish the National Program to Advance Artificial Intelligence Research, to promote research on artificial intelligence at the National Science Foundation, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>2020-06-04</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3891/2019</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3891/all-info</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Cory Gardner</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>HB2575</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>AI in Government Act of 2020</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Establishes the AI Center of Excellence within the General Services Administration to advise and promote the efforts of the federal government in developing innovative uses of artificial intelligence (AI) to benefit the public, and improve cohesion and competency in the use of AI. The Office of Management and Budget must issue a memorandum to federal agencies regarding AI governance approaches, to be followed by preparation and submission of governance plans by the agencies. In addition, the Office of Personnel Management must identify key skills and competencies needed for positions related to AI; and establish an occupational series, or revise an existing job series, to include positions the primary duties of which relate to AI.</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>2</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>2020-09-15</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2575/2019</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/2575/all-info</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>Jerry McNerney</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>SB3901</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>AI Scholarship-for-Service Act</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Establishes a federal artificial intelligence (AI) scholarship-for-service program to recruit and train AI professionals to lead and support AI in federal, state, local, and tribal governments. Specifically, the National Science Foundation must establish criteria to designate qualified institutions of higher education (IHEs) as eligible to participate in the program. Such criteria must include (1) measures of an IHE's demonstrated excellence in the education of students in AI; and (2) measures of an IHE's ability to attract and retain a diverse and nontraditional student population in science, technology, engineering, and mathematics. Further, the program must (1) provide scholarships through qualified IHEs to students who are enrolled in programs of study related to AI, (2) provide scholarship recipients with internship opportunities, (3) prioritize the employment placement of scholarship recipients in executive agencies, (4) identify opportunities to promote multidisciplinary programs of study that integrate basic or advanced AI training with other fields of study, and (5) support education research programs to train AI researchers and practitioners. Additionally, the post-award employment obligations of a scholarship recipient must include three years of work for an executive agency; Congress; an interstate agency; a state, local, or tribal government; or a government-affiliated nonprofit that is considered to be critical infrastructure. A scholarship recipient who completes less than the required three years of service must repay the scholarship, or the scholarship must be treated as a Federal Direct Unsubsidized Stafford Loan that is subject to repayment.</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>2020-06-04</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3901/2019</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3901/all-info</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Gary Peters</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>HB617</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Department of Energy Veterans' Health Initiative Act</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Directs the Department of Energy (DOE) to establish a research program in artificial intelligence and high-performance computing that is focused on the development of tools to (1) solve big data challenges associated with veterans' health care, and (2) support the Department of Veterans Affairs in identifying potential health risks and challenges. DOE may carry out research and development activities to develop tools to apply to big data that enable federal agencies, institutions of higher education, nonprofit research organizations, and industry to better leverage the capabilities of DOE to solve complex, big data challenges.</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>2</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>2019-07-24</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB617/2019</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/617/all-info</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>Ralph Norman</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>HB7096</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>National AI Research Resource Task Force Act of 2020</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>To establish the National Artificial Intelligence Research Resource Task Force, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>1</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>2020-06-04</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7096/2019</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/7096/all-info</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>Anna Eshoo</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>HB8230</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Integrating New Technologies to Empower Law Enforcement at Our Borders Act</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Requires the Department of Homeland Security to report to Congress a plan to identify and deploy emerging and advanced technologies (e.g. artificial intelligence, automation, and optical radar) to achieve greater situational awareness along the northern and southern U.S. borders between ports of entry. The report shall contain information including assessments of (1) how Customs and Border Protection is currently using such technologies, (2) how such technologies can address border security capability gaps, and (3) the cost of acquiring such technologies.</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>2020-09-11</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB8230/2019</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/8230/all-info</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>Elissa Slotkin</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>SB3832</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Endless Frontier Act</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Redesignates the National Science Foundation as the National Science and Technology Foundation and establishes a Directorate for Technology within the foundation. The goals of the directorate shall be to (1) strengthen U.S. leadership in critical technologies through fundamental research in key technology focus areas, such as artificial intelligence, high-performance computing, and advanced manufacturing; (2) enhance U.S. competitiveness in the focus areas by improving education in such areas and attracting more students to such areas; and (3) foster the impact of federally funded research and development through accelerated translation of advances in the focus areas into processes and products that help achieve national goals. The Department of Commerce shall carry out a program to designate and support eligible consortia as regional technology hubs that facilitate activities that (1) enable U.S. leadership in a key technology focus area, and (2) support regional economic development that diffuses innovation capacity around the United States. The Office of Science and Technology Policy, Commerce, the National Security Council, and other relevant federal agencies shall (1) review the national security strategy and programs and resources pertaining to U.S. national competitiveness in science, research, and innovation to support such strategy; and (2) develop a strategy for the federal government to improve such competitiveness to support the national security strategy.</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>2020-05-21</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3832/2019</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3832/all-info</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>Charles Schumer</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>HB6829</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>EMPIL–DOC Act Expanding Medical Partnerships with Israel to Lessen Dependence on China Act</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Authorizes a bilateral grant program with Israel to develop health technologies, with an emphasis on the use of technology, personalized medicine, and data in relation to COVID-19 (i.e., coronavirus disease 2019). Technologies to be developed through this program include, among others, artificial intelligence, respiratory assist devices, and diagnostic tests. In addition, the program conditions funding on a matching contribution from the government of Israel.</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>1</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>2020-05-12</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6829/2019</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6829/all-info</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>Christopher Pappas</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>SB3890</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>National AI Research Resource Task Force Act of 2020</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>A bill to establish the National Artificial Intelligence Research Resource Task Force, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>2020-06-04</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3890/2019</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3890/all-info</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>Rob Portman</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>HB6937</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Countering Online Harms Act</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Requires the Federal Trade Commission to study and report on how artificial intelligence may be used to identify, remove, and take action to address online harms, including (1) scams directed at older adults; (2) intentionally misleading content; (3) disinformation campaigns to influence elections; and (3) content furthering other illegal activity such as the sale of opioids, child sexual exploitation, terrorism, and the sale of counterfeit products.</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>2020-05-19</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6937/2019</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6937/all-info</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>Brett Guthrie</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>SB3771</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>FUTURE of Artificial Intelligence Act of 2020 Fundamentally Understanding the Usability and Realistic Evolution of Artificial Intelligence Act of 2020</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>A bill to require the Secretary of Commerce to establish the Federal Advisory Committee on the Development and Implementation of Artificial Intelligence, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>1</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>2020-05-20</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3771/2019</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/3771/all-info</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>Maria Cantwell</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>HB3600</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Deepfakes Report Act of 2019</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Requires the Science and Technology Directorate in the Department of Homeland Security to report at specified intervals on the state of digital content forgery technology. Digital content forgery is the use of emerging technologies, including artificial intelligence and machine learning techniques, to fabricate or manipulate audio, visual, or text content with the intent to mislead.</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>1</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>2019-06-28</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB3600/2019</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/3600/all-info</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>Derek Kilmer</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>HCR116</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Expressing the sense of Congress with respect to the principles that should guide the national artificial intelligence strategy of the United States.</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>This concurrent resolution sets forth considerations for Congress in guiding the national artificial intelligence strategy. Specifically, the resolution, among other things, expresses the sense of Congress that the United States should take a global leadership role in artificial intelligence; the federal government should increase funding for existing technology education programs; the United States should leverage its alliances to promote democratic principles, foster research collaboration, and develop common standards with respect to artificial intelligence; and the federal government should increase investments in artificial intelligence research and development and related fields.</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>1</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>2020-09-16</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HCR116/2019</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-concurrent-resolution/116/all-info</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Will Hurd</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>SB4082</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence Standards and National Security Act</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Requires the Department of Defense (DOD) to submit certain reports with respect to artificial intelligence. Specifically, DOD must report to Congress on the role of DOD in the development of artificial intelligence standards, including an assessment of the ways in which an artificial intelligence standards strategy will improve the national security; and the feasibility and current status of assigning members of the Armed Forces on active duty to the Joint Artificial Intelligence Center of DOD.</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>1</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>2020-06-25</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB4082/2019</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/4082/all-info</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>Michael Bennet</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>HB8390</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>To require the Director of the National Science Foundation to establish a grant program to make grants to eligible entities to develop instructional content on artificial intelligence, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>To require the Director of the National Science Foundation to establish a grant program to make grants to eligible entities to develop instructional content on artificial intelligence, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>1</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>2020-09-24</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB8390/2019</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/8390/all-info</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>Paul Tonko</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>HB2231</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Algorithmic Accountability Act of 2019</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Requires specified commercial entities to conduct assessments of high-risk systems that involve personal information or make automated decisions, such as systems that use artificial intelligence or machine learning.Specifically, high-risk automated decision systems include those that (1) may contribute to inaccuracy, bias, or discrimination; or (2) facilitate decision-making about sensitive aspects of consumers' lives by evaluating consumers' behavior. Further, an automated-decision system, or information system involving personal data, is considered high-risk if it (1) raises security or privacy concerns, (2) involves the personal information of a significant number of people, or (3) systematically monitors a large, publicly accessible physical location.Assessments of high-risk automated-decision systems must (1) describe the system in detail, (2) assess the relative costs and benefits of the system, (3) determine the risks to the privacy and security of personal information, and (4) explain the steps taken to minimize those risks, if discovered. Assessments of high-risk information systems involving personal information must evaluate the extent to which the system protects the privacy and security of such information.</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>1</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>2019-04-10</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2231/2019</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/2231/all-info</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>Yvette Clarke</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>HB8128</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Consumer Safety Technology Act</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Requires various agencies to explore the use of emerging technologies in the context of consumer products and safety. First, the Consumer Product and Safety Commission must consult with relevant stakeholders, such as data scientists and product manufacturers, and use artificial intelligence in a pilot program for a least one of the following processes: (1) tracking trends in injuries involving consumer products, (2) identifying consumer product hazards, (3) monitoring the sale of recalled consumer products, or (4) identifying consumer products that do not meet specified importation requirements related to product safety. Additionally, the Department of Commerce must consult with the Federal Trade Commission (FTC) and other relevant agencies to study potential applications of blockchain technology (i.e., the technology that supports digital currencies such as Bitcoin), including the use of such technology to address fraud and other unfair or deceptive practices. Finally, the FTC must report on its efforts to address unfair or deceptive trade practices related to digital tokens (i.e., transferable units of a digital currency).</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>2</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB8128/2019</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/8128/all-info</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Jerry McNerney</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>HB827</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>AI JOBS Act of 2019 Artificial Intelligence Job Opportunities and Background Summary Act of 2019</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Expresses the sense of Congress that technology can improve the lives of individuals, but can also disrupt jobs, and for this reason, innovation should be encouraged while training and retraining American workers. The Department of Labor shall prepare and submit to Congress a report on artificial intelligence and its impact on the workforce.</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>1</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>2019-01-28</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB827/2019</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/827/all-info</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>Darren Soto</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>SB4200</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Information Technology Modernization Centers of Excellence Program Act</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Requires the General Service Administration (GSA) to establish an Information Technology Modernization Centers of Excellence Program to facilitate the adoption of modern technology by executive agencies. The bill lists program responsibilities, including to modernize information technology used by an executive agency and how a customer interacts with the agency; improve cooperation between commercial and executive agency information technology sectors; encourage the adoption of commercial items; and assist executive agencies, on a reimbursable basis, with planning and adoption of technology in focus areas designated by the GSA, which may include, among other things, artificial intelligence. The GSA, for each reimbursable agreement entered into, shall make specified information available on a public website within 30 days of the signing of the agreement and updated upon completion. shall sunset seven years after its enactment.</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>1</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>2020-07-02</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB4200/2019</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/4200/all-info</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>Rob Portman</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>SB2065</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Deepfake Report Act of 2019</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Requires the Science and Technology Directorate in the Department of Homeland Security to report at specified intervals on the state of digital content forgery technology. Digital content forgery is the use of emerging technologies, including artificial intelligence and machine learning techniques, to fabricate or manipulate audio, visual, or text content with the intent to mislead.</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>2</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>2019-10-28</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2065/2019</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/senate-bill/2065/all-info</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>Rob Portman</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>HB6950</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>GAINS Act Generating Artificial Intelligence Networking Security Act</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Requires the Department of Commerce to study and report on the impact of artificial intelligence, including machine learning, on U.S. businesses conducting interstate commerce. Such study shall involve, among other things, (1) listing industry sectors that develop and use artificial intelligence and public-private partnerships focused on promoting the adoption and use of such technology, (2) establishing a list of federal agencies asserting jurisdiction over such industry sectors and entities and determining how these agencies are reducing barriers to business adoption and use of artificial intelligence, and (3) assessing risks and trends in the marketplace and supply chain of artificial intelligence. Commerce must report to Congress the results of such study and any recommendations to promote the adoption of artificial intelligence.</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>1</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>2020-05-19</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6950/2019</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6950/all-info</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>Cathy McMorris Rodgers</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>HB6395</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>William M. (Mac) Thornberry National Defense Authorization Act for Fiscal Year 2021</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Authorizes FY2021 appropriations and sets forth policies for Department of Defense (DOD) programs and activities, including military personnel strengths. It does not provide budget authority, which is provided in subsequent appropriations legislation. The bill authorizes appropriations to DOD for Procurement, including aircraft, weapons and tracked combat vehicles, shipbuilding and conversion, and missiles; Research, Development, Test, and Evaluation; Operation and Maintenance; Working Capital Funds; Chemical Agents and Munitions Destruction; Drug Interdiction and Counter-Drug Activities; the Defense Inspector General; the National Defense Sealift Fund; the Defense Health Program; the Armed Forces Retirement Home; the Space Force; Overseas Contingency Operations; and Military Construction. The bill also authorizes the FY2021 personnel strengths for active duty and reserve forces and sets forth policies regarding military personnel; acquisition policy and management; international programs; National Guard and Reserve Force facilities; compensation and other personnel benefits; health care; matters relating to COVID-19 (i.e., coronavirus disease 2019); DOD organization and management; civilian personnel matters; matters relating to foreign nations; and strategic programs, cyber, and intelligence matters. The bill authorizes appropriations for base realignment and closure activities, and maritime matters. The bill authorizes appropriations and sets forth policies for Department of Energy national security programs, including the National Nuclear Security Administration and the Defense Nuclear Facilities Safety Board. The bill also sets forth policies regarding certain federal activities related to artificial intelligence, including implementation by the President of a National Artificial Intelligence Initiative to support research and development, education, and training programs.</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>4</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6395/2019</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/6395/all-info</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Adam Smith</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>HB8763</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>To direct the Director of National Intelligence to award contracts or grants, or enter into transactions other than contracts, to encourage microelectronics research in support of artificial intelligence.</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Requires the Office of the Director of National Intelligence to enter into transactions, such as by awarding contracts or grants, to encourage microelectronics research.</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>1</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>2020-11-17</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB8763/2019</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/8763/all-info</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>Raja Krishnamoorthi</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>HB8132</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>American COMPETE Act American Competitiveness Of a More Productive Emerging Tech Economy Act</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Requires the Department of Commerce and the Federal Trade Commission to study and submit reports on the state of specified technology industries (e.g., artificial intelligence, quantum computing, blockchain technology, and unmanned delivery services) and the impact of these industries on the U.S. economy.</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>2</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB8132/2019</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/116th-congress/house-bill/8132/all-info</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>Cathy McMorris Rodgers</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>HB6553</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>AI JOBS Act of 2022 Artificial Intelligence Job Opportunities and Background Summary Act of 2022</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>To promote a 21st century artificial intelligence workforce.</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>1</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>2022-02-01</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB6553/2021</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/6553/all-info</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>Darren Soto</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>SB3175</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Advancing American Artificial Intelligence Innovation Act of 2021</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>A bill to authorize the Secretary of Defense to carry out a pilot program on establishing data libraries for training artificial intelligence models, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>1</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>2021-11-04</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3175/2021</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/3175/all-info</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>Jacky Rosen</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>HB5148</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>United States–Israel Artificial Intelligence Center Act</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>To establish the United States-Israel Artificial Intelligence Center to improve artificial intelligence research and development cooperation.</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>1</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>2021-09-03</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB5148/2021</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/5148/all-info</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>Jake Auchincloss</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>SB1353</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Advancing American AI Act</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>A bill to promote United States values and fulfill agency missions through the use of innovative applied artificial intelligence technologies, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>1</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>2021-04-22</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1353/2021</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/1353/all-info</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>Gary Peters</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>SB1257</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>AI Scholarship-for-Service Act</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>A bill to establish a Federal artificial intelligence scholarship-for-service program.</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>1</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>2021-04-20</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1257/2021</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/1257/all-info</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>Gary Peters</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>HB5467</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Healthy Technology Act of 2021</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>To amend the Federal Food, Drug, and Cosmetic Act to clarify that artificial intelligence and machine learning technologies can qualify as a practitioner eligible to prescribe drugs if authorized by the State involved and approved, cleared, or authorized by the Food and Drug Administration, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>1</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>2021-09-30</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB5467/2021</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/5467/all-info</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>David Schweikert</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>SB2904</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Department of Defense Artificial Intelligence Metrics Act of 2021</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>A bill to require the Secretary of Defense to establish performance objectives and accompanying metrics for the incorporation of artificial intelligence and digital readiness into Department of Defense platforms, processes, and operations, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>1</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>2021-09-30</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2904/2021</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/2904/all-info</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>Mike Rounds</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>HB2989</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Financial Transparency Act of 2021</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>To amend securities and banking laws to make the information reported to financial regulatory agencies electronically searchable, to further enable the development of RegTech and Artificial Intelligence applications, to put the United States on a path towards building a comprehensive Standard Business Reporting program to ultimately harmonize and reduce the private sector’s regulatory compliance burden, while enhancing transparency and accountability, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>2</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>2021-10-26</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB2989/2021</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/2989/all-info</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>Carolyn Maloney</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>HB7683</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>AI Training Act Artificial Intelligence Training for the Acquisition Workforce Act</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>To require the Director of the Office of Management and Budget to establish or otherwise provide an artificial intelligence training program for the acquisition workforce, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>1</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>2022-05-06</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7683/2021</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/7683/all-info</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>Carolyn Maloney</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>SB1705</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>AICT Act of 2021 Artificial Intelligence Capabilities and Transparency Act of 2021</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>A bill to establish a coordinated Federal initiative to accelerate the research, development, procurement, fielding, and sustainment of artificial intelligence for the economic and national security interests of the United States, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>1</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>2021-05-19</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1705/2021</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/1705/all-info</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>Martin Heinrich</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>HB3844</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Fellowships and Traineeships for Early-Career AI Researchers Act</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>To support fellowships and traineeships for early-career artificial intelligence researchers, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>1</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>2021-06-11</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB3844/2021</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/3844/all-info</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>Jay Obernolte</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>HB4985</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Digital Defense Leadership Act</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>To implement certain recommendations of the National Security Commission on Artificial Intelligence.</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>1</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>2021-08-06</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB4985/2021</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/4985/all-info</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>Filemon Vela</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>HB7296</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>GOOD AI Act of 2022 Government Ownership and Oversight of Data in Artificial Intelligence Act of 2022</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>To establish the Artificial Intelligence Hygiene Working Group, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>1</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>2022-03-30</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB7296/2021</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/7296/all-info</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>Brenda Lawrence</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>SB3035</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>GOOD AI Act of 2021 Government Ownership and Oversight of Data in Artificial Intelligence Act of 2021</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>A bill to establish the Artificial Intelligence Hygiene Working Group, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>1</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>2021-10-21</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB3035/2021</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/3035/all-info</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Gary Peters</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>HB3723</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>AI for Consumer Product Safety Act Blockchain Innovation Act Digital Taxonomy Act</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>To direct the Consumer Product Safety Commission to establish a pilot program to explore the use of artificial intelligence in support of the mission of the Commission and direct the Secretary of Commerce and the Federal Trade Commission to study and report on the use of blockchain technology and digital tokens, respectively.</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>2</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>2021-06-24</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB3723/2021</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/3723/all-info</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>Jerry McNerney</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>SB1776</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence for the Military Act of 2021</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>A bill to implement recommendations relating to military training on emerging technologies.</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>1</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>2021-05-20</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB1776/2021</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/1776/all-info</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>Rob Portman</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>HB4468</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>AI for Agency Impact Act Artificial Intelligence for Agency Impact Act</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>To amend chapter 3 of title 5, United States Code, to require Executive agencies to establish and implement an AI strategy, objectives, and metrics plan for trustworthy artificial intelligence adoption to better achieve the missions of such agencies to serve the people of the United States, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>1</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>2021-07-16</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB4468/2021</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/4468/all-info</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>Carolyn Maloney</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>SB2551</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>AI Training Act Artificial Intelligence Training for the Acquisition Workforce Act</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>A bill to require the Director of the Office of Management and Budget to establish or otherwise provide an artificial intelligence training program for the acquisition workforce, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>4</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>2022-10-17</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2551/2021</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/2551/all-info</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>Gary Peters</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>SB4295</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Financial Data Transparency Act of 2022</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>A bill to amend securities and banking laws to make the information reported to financial regulatory agencies electronically searchable, to further enable the development of regulatory technologies and artificial intelligence applications, to put the United States on a path towards building a comprehensive Standard Business Reporting program to ultimately harmonize and reduce the private sector's regulatory compliance burden, while enhancing transparency and accountability, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>1</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>2022-05-24</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB4295/2021</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/4295/all-info</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>Mark Warner</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>SB2120</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>United States–Israel Artificial Intelligence Center Act</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>A bill to establish the United States-Israel Artificial Intelligence Center to improve artificial intelligence research and development cooperation.</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>1</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>2021-06-17</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/SB2120/2021</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/senate-bill/2120/all-info</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>Marco Rubio</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>HB4469</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>AI in Counterterrorism Oversight Enhancement Act</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>To amend the Intelligence Reform and Terrorism Prevention Act of 2004 to strengthen the ability of the Privacy and Civil Liberties Oversight Board to provide meaningful oversight and governance related to the use of artificial intelligence technologies for counterterrorism purposes, and for other purposes.</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>1</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>2021-07-16</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>https://legiscan.com/US/bill/HB4469/2021</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>https://www.congress.gov/bill/117th-congress/house-bill/4469/all-info</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>Carolyn Maloney</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>